<commit_message>
Updated Excell and Started Q2
</commit_message>
<xml_diff>
--- a/TCP23_data.xlsx
+++ b/TCP23_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charles.scheuermann/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charles.scheuermann/Documents/GitHub/E-Bikes-M3-Challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673538E1-B5FF-F74A-B735-C0C74EAF11BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB96303-491A-DF49-A856-2FE61298C4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q1 E-bike Sales" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="133">
   <si>
     <t>E-bike Sales Data Across the World</t>
   </si>
@@ -712,6 +712,18 @@
       <t>https://www.gov.uk/government/statistical-data-sets/tsgb01-modal-comparisons#passenger-transport</t>
     </r>
   </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Battery Cost (US$/kW-hr)</t>
+  </si>
+  <si>
+    <t>Battery Gravimetric Energy Densities (W-hr/kg)</t>
+  </si>
+  <si>
+    <t>% People Considering Climate as Top 3 Issue</t>
+  </si>
 </sst>
 </file>
 
@@ -1135,6 +1147,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1155,9 +1170,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1394,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R1003"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -2990,10 +3002,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z993"/>
+  <dimension ref="A1:AF993"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="O3" workbookViewId="0">
+      <selection activeCell="Z16" sqref="Z16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -3013,8 +3025,8 @@
     <col min="13" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="17">
-      <c r="A1" s="89">
+    <row r="1" spans="1:32" ht="17">
+      <c r="A1" s="90">
         <v>1</v>
       </c>
       <c r="B1" s="85"/>
@@ -3024,8 +3036,8 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="45" customHeight="1">
-      <c r="A2" s="90" t="s">
+    <row r="2" spans="1:32" ht="45" customHeight="1">
+      <c r="A2" s="91" t="s">
         <v>22</v>
       </c>
       <c r="B2" s="87"/>
@@ -3036,8 +3048,8 @@
       <c r="G2" s="87"/>
       <c r="H2" s="87"/>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="95"/>
+    <row r="3" spans="1:32" ht="14.25" customHeight="1">
+      <c r="A3" s="96"/>
       <c r="B3" s="85"/>
       <c r="C3" s="85"/>
       <c r="D3" s="85"/>
@@ -3045,8 +3057,11 @@
       <c r="F3" s="85"/>
       <c r="G3" s="85"/>
       <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="S3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="14.25" customHeight="1">
       <c r="A4" s="15" t="s">
         <v>23</v>
       </c>
@@ -3076,7 +3091,7 @@
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+    <row r="5" spans="1:32" ht="14.25" customHeight="1">
       <c r="A5" s="16"/>
       <c r="B5" s="72" t="s">
         <v>24</v>
@@ -3106,7 +3121,7 @@
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+    <row r="6" spans="1:32" ht="14.25" customHeight="1">
       <c r="A6" s="16"/>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
@@ -3125,16 +3140,28 @@
       <c r="P6" s="7"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
       <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
       <c r="Z6" s="7"/>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA6" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB6" s="77" t="s">
+        <v>130</v>
+      </c>
+      <c r="AC6" s="77" t="s">
+        <v>131</v>
+      </c>
+      <c r="AD6" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE6" s="71" t="s">
+        <v>132</v>
+      </c>
+      <c r="AF6" s="74" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" ht="14.25" customHeight="1">
       <c r="A7" s="16"/>
       <c r="B7" s="19" t="s">
         <v>25</v>
@@ -3157,16 +3184,17 @@
       <c r="P7" s="7"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
       <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
       <c r="Z7" s="7"/>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA7" s="33">
+        <v>1991</v>
+      </c>
+      <c r="AB7" s="78"/>
+      <c r="AC7" s="33">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" ht="14.25" customHeight="1">
       <c r="A8" s="16"/>
       <c r="B8" s="20" t="s">
         <v>27</v>
@@ -3197,16 +3225,18 @@
       <c r="P8" s="7"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
       <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA8" s="33">
+        <v>1992</v>
+      </c>
+      <c r="AB8" s="78"/>
+      <c r="AC8" s="78"/>
+      <c r="AD8" s="43">
+        <v>1.087</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" ht="14.25" customHeight="1">
       <c r="A9" s="16"/>
       <c r="B9" s="16" t="s">
         <v>32</v>
@@ -3237,16 +3267,18 @@
       <c r="P9" s="7"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
-      <c r="S9" s="7"/>
-      <c r="T9" s="7"/>
       <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="7"/>
       <c r="Z9" s="7"/>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA9" s="33">
+        <v>1993</v>
+      </c>
+      <c r="AB9" s="78"/>
+      <c r="AC9" s="78"/>
+      <c r="AD9" s="43">
+        <v>1.0669999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" ht="14.25" customHeight="1">
       <c r="A10" s="16"/>
       <c r="B10" s="16" t="s">
         <v>34</v>
@@ -3277,16 +3309,20 @@
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
-      <c r="S10" s="7"/>
-      <c r="T10" s="7"/>
       <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="7"/>
       <c r="Z10" s="7"/>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA10" s="33">
+        <v>1994</v>
+      </c>
+      <c r="AB10" s="78"/>
+      <c r="AC10" s="33">
+        <v>105</v>
+      </c>
+      <c r="AD10" s="43">
+        <v>1.075</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" ht="14.25" customHeight="1">
       <c r="A11" s="16"/>
       <c r="B11" s="16" t="s">
         <v>36</v>
@@ -3317,16 +3353,22 @@
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
-      <c r="S11" s="7"/>
-      <c r="T11" s="7"/>
       <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
-      <c r="X11" s="7"/>
-      <c r="Y11" s="7"/>
       <c r="Z11" s="7"/>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA11" s="33">
+        <v>1995</v>
+      </c>
+      <c r="AB11" s="33">
+        <v>3200</v>
+      </c>
+      <c r="AC11" s="33">
+        <v>110</v>
+      </c>
+      <c r="AD11" s="43">
+        <v>1.111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" ht="14.25" customHeight="1">
       <c r="A12" s="16"/>
       <c r="B12" s="16" t="s">
         <v>38</v>
@@ -3357,16 +3399,20 @@
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
       <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA12" s="33">
+        <v>1996</v>
+      </c>
+      <c r="AB12" s="78"/>
+      <c r="AC12" s="33">
+        <v>125</v>
+      </c>
+      <c r="AD12" s="43">
+        <v>1.1990000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" ht="14.25" customHeight="1">
       <c r="A13" s="16"/>
       <c r="B13" s="16" t="s">
         <v>40</v>
@@ -3397,16 +3443,20 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
-      <c r="S13" s="7"/>
-      <c r="T13" s="7"/>
       <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="7"/>
       <c r="Z13" s="7"/>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA13" s="33">
+        <v>1997</v>
+      </c>
+      <c r="AB13" s="33">
+        <v>2500</v>
+      </c>
+      <c r="AC13" s="78"/>
+      <c r="AD13" s="43">
+        <v>1.1990000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" ht="14.25" customHeight="1">
       <c r="A14" s="16"/>
       <c r="B14" s="16" t="s">
         <v>42</v>
@@ -3437,16 +3487,20 @@
       <c r="P14" s="7"/>
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
-      <c r="S14" s="7"/>
-      <c r="T14" s="7"/>
       <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
-      <c r="Y14" s="7"/>
       <c r="Z14" s="7"/>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA14" s="33">
+        <v>1998</v>
+      </c>
+      <c r="AB14" s="78"/>
+      <c r="AC14" s="33">
+        <v>140</v>
+      </c>
+      <c r="AD14" s="43">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" ht="14.25" customHeight="1">
       <c r="A15" s="16"/>
       <c r="B15" s="16" t="s">
         <v>44</v>
@@ -3471,16 +3525,20 @@
       <c r="P15" s="7"/>
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
       <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="7"/>
       <c r="Z15" s="7"/>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA15" s="33">
+        <v>1999</v>
+      </c>
+      <c r="AB15" s="33">
+        <v>1800</v>
+      </c>
+      <c r="AC15" s="78"/>
+      <c r="AD15" s="43">
+        <v>1.1359999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" ht="14.25" customHeight="1">
       <c r="A16" s="16"/>
       <c r="B16" s="16" t="s">
         <v>45</v>
@@ -3505,16 +3563,23 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
       <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="7"/>
       <c r="Z16" s="7"/>
-    </row>
-    <row r="17" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA16" s="33">
+        <v>2000</v>
+      </c>
+      <c r="AB16" s="78"/>
+      <c r="AC16" s="33">
+        <v>150</v>
+      </c>
+      <c r="AD16" s="43">
+        <v>1.484</v>
+      </c>
+      <c r="AF16" s="32">
+        <v>33645</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" ht="14.25" customHeight="1">
       <c r="A17" s="16"/>
       <c r="B17" s="16" t="s">
         <v>46</v>
@@ -3539,16 +3604,23 @@
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
       <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
-      <c r="Y17" s="7"/>
       <c r="Z17" s="7"/>
-    </row>
-    <row r="18" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA17" s="33">
+        <v>2001</v>
+      </c>
+      <c r="AB17" s="78"/>
+      <c r="AC17" s="33">
+        <v>155</v>
+      </c>
+      <c r="AD17" s="43">
+        <v>1.42</v>
+      </c>
+      <c r="AF17" s="32">
+        <v>34216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" ht="14.25" customHeight="1">
       <c r="A18" s="16"/>
       <c r="B18" s="16" t="s">
         <v>47</v>
@@ -3573,16 +3645,23 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
       <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="7"/>
       <c r="Z18" s="7"/>
-    </row>
-    <row r="19" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA18" s="33">
+        <v>2002</v>
+      </c>
+      <c r="AB18" s="78"/>
+      <c r="AC18" s="33">
+        <v>165</v>
+      </c>
+      <c r="AD18" s="43">
+        <v>1.345</v>
+      </c>
+      <c r="AF18" s="32">
+        <v>34894</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" ht="14.25" customHeight="1">
       <c r="A19" s="16"/>
       <c r="B19" s="16" t="s">
         <v>48</v>
@@ -3607,16 +3686,23 @@
       <c r="P19" s="7"/>
       <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
       <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
-      <c r="Y19" s="7"/>
       <c r="Z19" s="7"/>
-    </row>
-    <row r="20" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA19" s="33">
+        <v>2003</v>
+      </c>
+      <c r="AB19" s="33">
+        <v>830</v>
+      </c>
+      <c r="AC19" s="78"/>
+      <c r="AD19" s="43">
+        <v>1.5609999999999999</v>
+      </c>
+      <c r="AF19" s="32">
+        <v>35474</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" ht="14.25" customHeight="1">
       <c r="A20" s="16"/>
       <c r="B20" s="16" t="s">
         <v>49</v>
@@ -3641,16 +3727,23 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="7"/>
       <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
       <c r="U20" s="7"/>
-      <c r="V20" s="7"/>
-      <c r="W20" s="7"/>
-      <c r="X20" s="7"/>
-      <c r="Y20" s="7"/>
       <c r="Z20" s="7"/>
-    </row>
-    <row r="21" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA20" s="33">
+        <v>2004</v>
+      </c>
+      <c r="AB20" s="78"/>
+      <c r="AC20" s="33">
+        <v>185</v>
+      </c>
+      <c r="AD20" s="43">
+        <v>1.8520000000000001</v>
+      </c>
+      <c r="AF20" s="32">
+        <v>36325</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" ht="14.25" customHeight="1">
       <c r="A21" s="16"/>
       <c r="B21" s="16" t="s">
         <v>50</v>
@@ -3675,16 +3768,29 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="7"/>
       <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
       <c r="U21" s="7"/>
       <c r="V21" s="7"/>
       <c r="W21" s="7"/>
       <c r="X21" s="7"/>
       <c r="Y21" s="7"/>
       <c r="Z21" s="7"/>
-    </row>
-    <row r="22" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA21" s="33">
+        <v>2005</v>
+      </c>
+      <c r="AB21" s="33">
+        <v>630</v>
+      </c>
+      <c r="AC21" s="33">
+        <v>195</v>
+      </c>
+      <c r="AD21" s="43">
+        <v>2.27</v>
+      </c>
+      <c r="AF21" s="32">
+        <v>36526</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" ht="14.25" customHeight="1">
       <c r="A22" s="16"/>
       <c r="B22" s="16" t="s">
         <v>51</v>
@@ -3709,16 +3815,25 @@
       <c r="P22" s="7"/>
       <c r="Q22" s="7"/>
       <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7"/>
       <c r="U22" s="7"/>
       <c r="V22" s="7"/>
       <c r="W22" s="7"/>
       <c r="X22" s="7"/>
       <c r="Y22" s="7"/>
       <c r="Z22" s="7"/>
-    </row>
-    <row r="23" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA22" s="33">
+        <v>2006</v>
+      </c>
+      <c r="AB22" s="78"/>
+      <c r="AC22" s="78"/>
+      <c r="AD22" s="43">
+        <v>2.5720000000000001</v>
+      </c>
+      <c r="AF22" s="32">
+        <v>37570</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" ht="14.25" customHeight="1">
       <c r="A23" s="16"/>
       <c r="B23" s="16" t="s">
         <v>52</v>
@@ -3743,16 +3858,25 @@
       <c r="P23" s="7"/>
       <c r="Q23" s="7"/>
       <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7"/>
       <c r="U23" s="7"/>
       <c r="V23" s="7"/>
       <c r="W23" s="7"/>
       <c r="X23" s="7"/>
       <c r="Y23" s="7"/>
       <c r="Z23" s="7"/>
-    </row>
-    <row r="24" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA23" s="33">
+        <v>2007</v>
+      </c>
+      <c r="AB23" s="78"/>
+      <c r="AC23" s="78"/>
+      <c r="AD23" s="43">
+        <v>2.7959999999999998</v>
+      </c>
+      <c r="AF23" s="32">
+        <v>38093</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" ht="14.25" customHeight="1">
       <c r="A24" s="16"/>
       <c r="B24" s="16" t="s">
         <v>53</v>
@@ -3777,16 +3901,27 @@
       <c r="P24" s="7"/>
       <c r="Q24" s="7"/>
       <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7"/>
       <c r="U24" s="7"/>
       <c r="V24" s="7"/>
       <c r="W24" s="7"/>
       <c r="X24" s="7"/>
       <c r="Y24" s="7"/>
       <c r="Z24" s="7"/>
-    </row>
-    <row r="25" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA24" s="33">
+        <v>2008</v>
+      </c>
+      <c r="AB24" s="78"/>
+      <c r="AC24" s="33">
+        <v>205</v>
+      </c>
+      <c r="AD24" s="43">
+        <v>3.246</v>
+      </c>
+      <c r="AF24" s="32">
+        <v>38188</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" ht="14.25" customHeight="1">
       <c r="A25" s="16"/>
       <c r="B25" s="16" t="s">
         <v>54</v>
@@ -3811,16 +3946,25 @@
       <c r="P25" s="7"/>
       <c r="Q25" s="7"/>
       <c r="R25" s="7"/>
-      <c r="S25" s="7"/>
-      <c r="T25" s="7"/>
       <c r="U25" s="7"/>
       <c r="V25" s="7"/>
       <c r="W25" s="7"/>
       <c r="X25" s="7"/>
       <c r="Y25" s="7"/>
       <c r="Z25" s="7"/>
-    </row>
-    <row r="26" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA25" s="33">
+        <v>2009</v>
+      </c>
+      <c r="AB25" s="78"/>
+      <c r="AC25" s="78"/>
+      <c r="AD25" s="43">
+        <v>2.3530000000000002</v>
+      </c>
+      <c r="AF25" s="32">
+        <v>37814</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" ht="14.25" customHeight="1">
       <c r="A26" s="16"/>
       <c r="B26" s="16" t="s">
         <v>55</v>
@@ -3845,16 +3989,27 @@
       <c r="P26" s="7"/>
       <c r="Q26" s="7"/>
       <c r="R26" s="7"/>
-      <c r="S26" s="7"/>
-      <c r="T26" s="7"/>
       <c r="U26" s="7"/>
       <c r="V26" s="7"/>
       <c r="W26" s="7"/>
       <c r="X26" s="7"/>
       <c r="Y26" s="7"/>
       <c r="Z26" s="7"/>
-    </row>
-    <row r="27" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA26" s="33">
+        <v>2010</v>
+      </c>
+      <c r="AB26" s="33">
+        <v>370</v>
+      </c>
+      <c r="AC26" s="78"/>
+      <c r="AD26" s="43">
+        <v>2.782</v>
+      </c>
+      <c r="AF26" s="32">
+        <v>38282</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" ht="14.25" customHeight="1">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -3873,16 +4028,28 @@
       <c r="P27" s="7"/>
       <c r="Q27" s="7"/>
       <c r="R27" s="7"/>
-      <c r="S27" s="7"/>
-      <c r="T27" s="7"/>
       <c r="U27" s="7"/>
       <c r="V27" s="7"/>
       <c r="W27" s="7"/>
       <c r="X27" s="7"/>
       <c r="Y27" s="7"/>
       <c r="Z27" s="7"/>
-    </row>
-    <row r="28" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA27" s="33">
+        <v>2011</v>
+      </c>
+      <c r="AB27" s="78"/>
+      <c r="AC27" s="78"/>
+      <c r="AD27" s="43">
+        <v>3.5209999999999999</v>
+      </c>
+      <c r="AE27" s="75">
+        <v>7</v>
+      </c>
+      <c r="AF27" s="32">
+        <v>38769</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" ht="14.25" customHeight="1">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -3901,16 +4068,28 @@
       <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
       <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
       <c r="U28" s="7"/>
       <c r="V28" s="7"/>
       <c r="W28" s="7"/>
       <c r="X28" s="7"/>
       <c r="Y28" s="7"/>
       <c r="Z28" s="7"/>
-    </row>
-    <row r="29" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA28" s="33">
+        <v>2012</v>
+      </c>
+      <c r="AB28" s="78"/>
+      <c r="AC28" s="78"/>
+      <c r="AD28" s="43">
+        <v>3.6179999999999999</v>
+      </c>
+      <c r="AE28" s="75">
+        <v>7</v>
+      </c>
+      <c r="AF28" s="32">
+        <v>39732</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" ht="14.25" customHeight="1">
       <c r="A29" s="16"/>
       <c r="B29" s="82" t="s">
         <v>56</v>
@@ -3939,8 +4118,24 @@
       <c r="X29" s="7"/>
       <c r="Y29" s="7"/>
       <c r="Z29" s="7"/>
-    </row>
-    <row r="30" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA29" s="33">
+        <v>2013</v>
+      </c>
+      <c r="AB29" s="78"/>
+      <c r="AC29" s="33">
+        <v>240</v>
+      </c>
+      <c r="AD29" s="43">
+        <v>3.5049999999999999</v>
+      </c>
+      <c r="AE29" s="75">
+        <v>7</v>
+      </c>
+      <c r="AF29" s="32">
+        <v>38947</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" ht="14.25" customHeight="1">
       <c r="A30" s="16"/>
       <c r="B30" s="16" t="s">
         <v>57</v>
@@ -3969,8 +4164,22 @@
       <c r="X30" s="7"/>
       <c r="Y30" s="7"/>
       <c r="Z30" s="7"/>
-    </row>
-    <row r="31" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA30" s="33">
+        <v>2014</v>
+      </c>
+      <c r="AB30" s="78"/>
+      <c r="AC30" s="78"/>
+      <c r="AD30" s="43">
+        <v>3.3580000000000001</v>
+      </c>
+      <c r="AE30" s="75">
+        <v>10</v>
+      </c>
+      <c r="AF30" s="32">
+        <v>40118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" ht="14.25" customHeight="1">
       <c r="A31" s="16"/>
       <c r="B31" s="82" t="s">
         <v>58</v>
@@ -3999,8 +4208,24 @@
       <c r="X31" s="7"/>
       <c r="Y31" s="7"/>
       <c r="Z31" s="7"/>
-    </row>
-    <row r="32" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA31" s="33">
+        <v>2015</v>
+      </c>
+      <c r="AB31" s="33">
+        <v>350</v>
+      </c>
+      <c r="AC31" s="78"/>
+      <c r="AD31" s="43">
+        <v>2.4289999999999998</v>
+      </c>
+      <c r="AE31" s="75">
+        <v>9</v>
+      </c>
+      <c r="AF31" s="32">
+        <v>41383</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" ht="14.25" customHeight="1">
       <c r="A32" s="16"/>
       <c r="B32" s="16" t="s">
         <v>59</v>
@@ -4029,8 +4254,20 @@
       <c r="X32" s="7"/>
       <c r="Y32" s="7"/>
       <c r="Z32" s="7"/>
-    </row>
-    <row r="33" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA32" s="33">
+        <v>2016</v>
+      </c>
+      <c r="AD32" s="43">
+        <v>2.1429999999999998</v>
+      </c>
+      <c r="AE32" s="75">
+        <v>9</v>
+      </c>
+      <c r="AF32" s="32">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" ht="14.25" customHeight="1">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16"/>
@@ -4057,14 +4294,38 @@
       <c r="X33" s="7"/>
       <c r="Y33" s="7"/>
       <c r="Z33" s="7"/>
-    </row>
-    <row r="34" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA33" s="33">
+        <v>2017</v>
+      </c>
+      <c r="AD33" s="43">
+        <v>2.415</v>
+      </c>
+      <c r="AE33" s="75">
+        <v>9</v>
+      </c>
+      <c r="AF33" s="32">
+        <v>42699</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" ht="14.25" customHeight="1">
       <c r="G34" s="22"/>
       <c r="H34" s="23"/>
       <c r="K34" s="24"/>
       <c r="L34" s="25"/>
-    </row>
-    <row r="35" spans="1:26" ht="19">
+      <c r="AA34" s="33">
+        <v>2018</v>
+      </c>
+      <c r="AD34" s="43">
+        <v>2.7189999999999999</v>
+      </c>
+      <c r="AE34" s="75">
+        <v>13</v>
+      </c>
+      <c r="AF34" s="32">
+        <v>43886</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" ht="19">
       <c r="A35" s="26" t="s">
         <v>60</v>
       </c>
@@ -4093,8 +4354,20 @@
       <c r="X35" s="7"/>
       <c r="Y35" s="7"/>
       <c r="Z35" s="7"/>
-    </row>
-    <row r="36" spans="1:26" ht="60" customHeight="1">
+      <c r="AA35" s="33">
+        <v>2019</v>
+      </c>
+      <c r="AD35" s="43">
+        <v>2.6040000000000001</v>
+      </c>
+      <c r="AE35" s="75">
+        <v>25</v>
+      </c>
+      <c r="AF35" s="32">
+        <v>44644</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" ht="60" customHeight="1">
       <c r="A36" s="27"/>
       <c r="B36" s="73" t="s">
         <v>10</v>
@@ -4127,8 +4400,20 @@
       <c r="X36" s="7"/>
       <c r="Y36" s="7"/>
       <c r="Z36" s="7"/>
-    </row>
-    <row r="37" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA36" s="33">
+        <v>2020</v>
+      </c>
+      <c r="AD36" s="43">
+        <v>2.1680000000000001</v>
+      </c>
+      <c r="AE36" s="75">
+        <v>25</v>
+      </c>
+      <c r="AF36" s="32">
+        <v>47241</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" ht="14.25" customHeight="1">
       <c r="A37" s="27"/>
       <c r="B37" s="27">
         <v>2000</v>
@@ -4161,8 +4446,20 @@
       <c r="X37" s="7"/>
       <c r="Y37" s="7"/>
       <c r="Z37" s="7"/>
-    </row>
-    <row r="38" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA37" s="33">
+        <v>2021</v>
+      </c>
+      <c r="AD37" s="43">
+        <v>3.008</v>
+      </c>
+      <c r="AE37" s="75">
+        <v>30</v>
+      </c>
+      <c r="AF37" s="32">
+        <v>48219</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" ht="14.25" customHeight="1">
       <c r="A38" s="27"/>
       <c r="B38" s="27">
         <v>2001</v>
@@ -4195,8 +4492,17 @@
       <c r="X38" s="7"/>
       <c r="Y38" s="7"/>
       <c r="Z38" s="7"/>
-    </row>
-    <row r="39" spans="1:26" ht="14.25" customHeight="1">
+      <c r="AA38" s="33">
+        <v>2022</v>
+      </c>
+      <c r="AD38" s="44">
+        <v>3.9510000000000001</v>
+      </c>
+      <c r="AE38" s="75">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" ht="14.25" customHeight="1">
       <c r="A39" s="27"/>
       <c r="B39" s="27">
         <v>2002</v>
@@ -4230,7 +4536,7 @@
       <c r="Y39" s="7"/>
       <c r="Z39" s="7"/>
     </row>
-    <row r="40" spans="1:26" ht="14.25" customHeight="1">
+    <row r="40" spans="1:32" ht="14.25" customHeight="1">
       <c r="A40" s="27"/>
       <c r="B40" s="27">
         <v>2003</v>
@@ -4264,7 +4570,7 @@
       <c r="Y40" s="7"/>
       <c r="Z40" s="7"/>
     </row>
-    <row r="41" spans="1:26" ht="14.25" customHeight="1">
+    <row r="41" spans="1:32" ht="14.25" customHeight="1">
       <c r="A41" s="27"/>
       <c r="B41" s="27">
         <v>2004</v>
@@ -4298,7 +4604,7 @@
       <c r="Y41" s="7"/>
       <c r="Z41" s="7"/>
     </row>
-    <row r="42" spans="1:26" ht="14.25" customHeight="1">
+    <row r="42" spans="1:32" ht="14.25" customHeight="1">
       <c r="A42" s="27"/>
       <c r="B42" s="27">
         <v>2005</v>
@@ -4332,7 +4638,7 @@
       <c r="Y42" s="7"/>
       <c r="Z42" s="7"/>
     </row>
-    <row r="43" spans="1:26" ht="14.25" customHeight="1">
+    <row r="43" spans="1:32" ht="14.25" customHeight="1">
       <c r="A43" s="27"/>
       <c r="B43" s="27">
         <v>2006</v>
@@ -4366,7 +4672,7 @@
       <c r="Y43" s="7"/>
       <c r="Z43" s="7"/>
     </row>
-    <row r="44" spans="1:26" ht="14.25" customHeight="1">
+    <row r="44" spans="1:32" ht="14.25" customHeight="1">
       <c r="A44" s="27"/>
       <c r="B44" s="27">
         <v>2007</v>
@@ -4400,7 +4706,7 @@
       <c r="Y44" s="7"/>
       <c r="Z44" s="7"/>
     </row>
-    <row r="45" spans="1:26" ht="14.25" customHeight="1">
+    <row r="45" spans="1:32" ht="14.25" customHeight="1">
       <c r="A45" s="27"/>
       <c r="B45" s="27">
         <v>2008</v>
@@ -4434,7 +4740,7 @@
       <c r="Y45" s="7"/>
       <c r="Z45" s="7"/>
     </row>
-    <row r="46" spans="1:26" ht="14.25" customHeight="1">
+    <row r="46" spans="1:32" ht="14.25" customHeight="1">
       <c r="A46" s="27"/>
       <c r="B46" s="27">
         <v>2009</v>
@@ -4468,7 +4774,7 @@
       <c r="Y46" s="7"/>
       <c r="Z46" s="7"/>
     </row>
-    <row r="47" spans="1:26" ht="14.25" customHeight="1">
+    <row r="47" spans="1:32" ht="14.25" customHeight="1">
       <c r="A47" s="27"/>
       <c r="B47" s="27">
         <v>2010</v>
@@ -4502,7 +4808,7 @@
       <c r="Y47" s="7"/>
       <c r="Z47" s="7"/>
     </row>
-    <row r="48" spans="1:26" ht="14.25" customHeight="1">
+    <row r="48" spans="1:32" ht="14.25" customHeight="1">
       <c r="A48" s="27"/>
       <c r="B48" s="27">
         <v>2011</v>
@@ -4906,7 +5212,7 @@
     </row>
     <row r="60" spans="1:26" ht="45" customHeight="1">
       <c r="A60" s="27"/>
-      <c r="B60" s="96" t="s">
+      <c r="B60" s="97" t="s">
         <v>63</v>
       </c>
       <c r="C60" s="85"/>
@@ -4936,7 +5242,7 @@
     </row>
     <row r="61" spans="1:26" ht="14.25" customHeight="1">
       <c r="A61" s="27"/>
-      <c r="B61" s="97"/>
+      <c r="B61" s="89"/>
       <c r="C61" s="85"/>
       <c r="D61" s="85"/>
       <c r="E61" s="85"/>
@@ -4994,7 +5300,7 @@
     </row>
     <row r="63" spans="1:26" ht="14.25" customHeight="1">
       <c r="A63" s="27"/>
-      <c r="B63" s="92" t="s">
+      <c r="B63" s="93" t="s">
         <v>65</v>
       </c>
       <c r="C63" s="85"/>
@@ -5123,20 +5429,20 @@
       <c r="B68" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="C68" s="91" t="s">
+      <c r="C68" s="92" t="s">
         <v>69</v>
       </c>
-      <c r="D68" s="91"/>
-      <c r="E68" s="91"/>
-      <c r="F68" s="91"/>
-      <c r="G68" s="91"/>
+      <c r="D68" s="92"/>
+      <c r="E68" s="92"/>
+      <c r="F68" s="92"/>
+      <c r="G68" s="92"/>
       <c r="H68" s="21"/>
-      <c r="I68" s="93" t="s">
+      <c r="I68" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="J68" s="94"/>
-      <c r="K68" s="94"/>
-      <c r="L68" s="94"/>
+      <c r="J68" s="95"/>
+      <c r="K68" s="95"/>
+      <c r="L68" s="95"/>
       <c r="M68" s="16"/>
       <c r="N68" s="7"/>
       <c r="O68" s="7"/>
@@ -6266,7 +6572,7 @@
     </row>
     <row r="98" spans="1:26" ht="45" customHeight="1">
       <c r="A98" s="27"/>
-      <c r="B98" s="97" t="s">
+      <c r="B98" s="89" t="s">
         <v>81</v>
       </c>
       <c r="C98" s="85"/>
@@ -10276,15 +10582,15 @@
     <row r="993" ht="14.25" customHeight="1"/>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="I68:L68"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="B60:G60"/>
+    <mergeCell ref="B61:G61"/>
     <mergeCell ref="B98:G98"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="C68:G68"/>
     <mergeCell ref="B63:G63"/>
-    <mergeCell ref="I68:L68"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="B60:G60"/>
-    <mergeCell ref="B61:G61"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B29" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -10342,7 +10648,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="16">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="90" t="s">
         <v>91</v>
       </c>
       <c r="B1" s="85"/>
@@ -10540,7 +10846,7 @@
       <c r="H14" s="63"/>
     </row>
     <row r="15" spans="1:28" ht="30" customHeight="1">
-      <c r="A15" s="95" t="s">
+      <c r="A15" s="96" t="s">
         <v>112</v>
       </c>
       <c r="B15" s="104"/>
@@ -15179,6 +15485,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100140DE9F585DC8F40B0E84E01E8517F06" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bc82e147d0e14d9399c913ef14ffa058">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="59ed0f22-5706-4746-b84b-503369b7a859" xmlns:ns3="3c9ee541-6375-4361-8ab6-60b6eb41dab8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c93d17706a2a581490681d1477857262" ns2:_="" ns3:_="">
     <xsd:import namespace="59ed0f22-5706-4746-b84b-503369b7a859"/>
@@ -15389,22 +15710,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F7BA688-880A-4116-AAFF-3D828EA460FF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C739518-0802-4EB4-9F3D-BC89C410C575}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4557CBC1-A3BE-42B2-A97B-4055186AF828}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15421,21 +15744,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C739518-0802-4EB4-9F3D-BC89C410C575}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F7BA688-880A-4116-AAFF-3D828EA460FF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
a bunch of work
</commit_message>
<xml_diff>
--- a/TCP23_data.xlsx
+++ b/TCP23_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charles.scheuermann/Documents/GitHub/E-Bikes-M3-Challenge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB96303-491A-DF49-A856-2FE61298C4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F62D0B-4EA8-BD4D-85AF-3C6ABA6DDA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="134">
   <si>
     <t>E-bike Sales Data Across the World</t>
   </si>
@@ -724,6 +724,9 @@
   <si>
     <t>% People Considering Climate as Top 3 Issue</t>
   </si>
+  <si>
+    <t>Bicycles - Billions of Passenger Miles</t>
+  </si>
 </sst>
 </file>
 
@@ -1406,8 +1409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R1003"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -3002,10 +3005,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AF993"/>
+  <dimension ref="A1:AG993"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="O3" workbookViewId="0">
-      <selection activeCell="Z16" sqref="Z16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AI3" sqref="AI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -3025,7 +3028,7 @@
     <col min="13" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="17">
+    <row r="1" spans="1:33" ht="97">
       <c r="A1" s="90">
         <v>1</v>
       </c>
@@ -3035,8 +3038,29 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:32" ht="45" customHeight="1">
+      <c r="AA1" s="77" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB1" s="77" t="s">
+        <v>130</v>
+      </c>
+      <c r="AC1" s="77" t="s">
+        <v>131</v>
+      </c>
+      <c r="AD1" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE1" s="71" t="s">
+        <v>132</v>
+      </c>
+      <c r="AF1" s="74" t="s">
+        <v>61</v>
+      </c>
+      <c r="AG1" s="68" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" ht="45" customHeight="1">
       <c r="A2" s="91" t="s">
         <v>22</v>
       </c>
@@ -3047,8 +3071,14 @@
       <c r="F2" s="87"/>
       <c r="G2" s="87"/>
       <c r="H2" s="87"/>
-    </row>
-    <row r="3" spans="1:32" ht="14.25" customHeight="1">
+      <c r="AA2">
+        <v>1990</v>
+      </c>
+      <c r="AG2" s="60">
+        <v>11.417999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="14.25" customHeight="1">
       <c r="A3" s="96"/>
       <c r="B3" s="85"/>
       <c r="C3" s="85"/>
@@ -3060,8 +3090,16 @@
       <c r="S3" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="4" spans="1:32" ht="14.25" customHeight="1">
+      <c r="AA3" s="33">
+        <v>1991</v>
+      </c>
+      <c r="AB3" s="78"/>
+      <c r="AC3" s="33">
+        <v>79</v>
+      </c>
+      <c r="AG3" s="60"/>
+    </row>
+    <row r="4" spans="1:33" ht="14.25" customHeight="1">
       <c r="A4" s="15" t="s">
         <v>23</v>
       </c>
@@ -3090,8 +3128,17 @@
       <c r="X4" s="7"/>
       <c r="Y4" s="7"/>
       <c r="Z4" s="7"/>
-    </row>
-    <row r="5" spans="1:32" ht="14.25" customHeight="1">
+      <c r="AA4" s="33">
+        <v>1992</v>
+      </c>
+      <c r="AB4" s="78"/>
+      <c r="AC4" s="78"/>
+      <c r="AD4" s="43">
+        <v>1.087</v>
+      </c>
+      <c r="AG4" s="60"/>
+    </row>
+    <row r="5" spans="1:33" ht="14.25" customHeight="1">
       <c r="A5" s="16"/>
       <c r="B5" s="72" t="s">
         <v>24</v>
@@ -3120,8 +3167,17 @@
       <c r="X5" s="7"/>
       <c r="Y5" s="7"/>
       <c r="Z5" s="7"/>
-    </row>
-    <row r="6" spans="1:32" ht="14.25" customHeight="1">
+      <c r="AA5" s="33">
+        <v>1993</v>
+      </c>
+      <c r="AB5" s="78"/>
+      <c r="AC5" s="78"/>
+      <c r="AD5" s="43">
+        <v>1.0669999999999999</v>
+      </c>
+      <c r="AG5" s="60"/>
+    </row>
+    <row r="6" spans="1:33" ht="14.25" customHeight="1">
       <c r="A6" s="16"/>
       <c r="B6" s="16"/>
       <c r="C6" s="16"/>
@@ -3142,26 +3198,19 @@
       <c r="R6" s="7"/>
       <c r="U6" s="7"/>
       <c r="Z6" s="7"/>
-      <c r="AA6" s="77" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB6" s="77" t="s">
-        <v>130</v>
-      </c>
-      <c r="AC6" s="77" t="s">
-        <v>131</v>
-      </c>
-      <c r="AD6" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="AE6" s="71" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF6" s="74" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:32" ht="14.25" customHeight="1">
+      <c r="AA6" s="33">
+        <v>1994</v>
+      </c>
+      <c r="AB6" s="78"/>
+      <c r="AC6" s="33">
+        <v>105</v>
+      </c>
+      <c r="AD6" s="43">
+        <v>1.075</v>
+      </c>
+      <c r="AG6" s="60"/>
+    </row>
+    <row r="7" spans="1:33" ht="14.25" customHeight="1">
       <c r="A7" s="16"/>
       <c r="B7" s="19" t="s">
         <v>25</v>
@@ -3187,14 +3236,22 @@
       <c r="U7" s="7"/>
       <c r="Z7" s="7"/>
       <c r="AA7" s="33">
-        <v>1991</v>
-      </c>
-      <c r="AB7" s="78"/>
+        <v>1995</v>
+      </c>
+      <c r="AB7" s="33">
+        <v>3200</v>
+      </c>
       <c r="AC7" s="33">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:32" ht="14.25" customHeight="1">
+        <v>110</v>
+      </c>
+      <c r="AD7" s="43">
+        <v>1.111</v>
+      </c>
+      <c r="AG7" s="60">
+        <v>10.821</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" ht="14.25" customHeight="1">
       <c r="A8" s="16"/>
       <c r="B8" s="20" t="s">
         <v>27</v>
@@ -3228,15 +3285,18 @@
       <c r="U8" s="7"/>
       <c r="Z8" s="7"/>
       <c r="AA8" s="33">
-        <v>1992</v>
+        <v>1996</v>
       </c>
       <c r="AB8" s="78"/>
-      <c r="AC8" s="78"/>
+      <c r="AC8" s="33">
+        <v>125</v>
+      </c>
       <c r="AD8" s="43">
-        <v>1.087</v>
-      </c>
-    </row>
-    <row r="9" spans="1:32" ht="14.25" customHeight="1">
+        <v>1.1990000000000001</v>
+      </c>
+      <c r="AG8" s="60"/>
+    </row>
+    <row r="9" spans="1:33" ht="14.25" customHeight="1">
       <c r="A9" s="16"/>
       <c r="B9" s="16" t="s">
         <v>32</v>
@@ -3270,15 +3330,18 @@
       <c r="U9" s="7"/>
       <c r="Z9" s="7"/>
       <c r="AA9" s="33">
-        <v>1993</v>
-      </c>
-      <c r="AB9" s="78"/>
+        <v>1997</v>
+      </c>
+      <c r="AB9" s="33">
+        <v>2500</v>
+      </c>
       <c r="AC9" s="78"/>
       <c r="AD9" s="43">
-        <v>1.0669999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:32" ht="14.25" customHeight="1">
+        <v>1.1990000000000001</v>
+      </c>
+      <c r="AG9" s="60"/>
+    </row>
+    <row r="10" spans="1:33" ht="14.25" customHeight="1">
       <c r="A10" s="16"/>
       <c r="B10" s="16" t="s">
         <v>34</v>
@@ -3312,17 +3375,18 @@
       <c r="U10" s="7"/>
       <c r="Z10" s="7"/>
       <c r="AA10" s="33">
-        <v>1994</v>
+        <v>1998</v>
       </c>
       <c r="AB10" s="78"/>
       <c r="AC10" s="33">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="AD10" s="43">
-        <v>1.075</v>
-      </c>
-    </row>
-    <row r="11" spans="1:32" ht="14.25" customHeight="1">
+        <v>1.03</v>
+      </c>
+      <c r="AG10" s="60"/>
+    </row>
+    <row r="11" spans="1:33" ht="14.25" customHeight="1">
       <c r="A11" s="16"/>
       <c r="B11" s="16" t="s">
         <v>36</v>
@@ -3356,19 +3420,18 @@
       <c r="U11" s="7"/>
       <c r="Z11" s="7"/>
       <c r="AA11" s="33">
-        <v>1995</v>
+        <v>1999</v>
       </c>
       <c r="AB11" s="33">
-        <v>3200</v>
-      </c>
-      <c r="AC11" s="33">
-        <v>110</v>
-      </c>
+        <v>1800</v>
+      </c>
+      <c r="AC11" s="78"/>
       <c r="AD11" s="43">
-        <v>1.111</v>
-      </c>
-    </row>
-    <row r="12" spans="1:32" ht="14.25" customHeight="1">
+        <v>1.1359999999999999</v>
+      </c>
+      <c r="AG11" s="60"/>
+    </row>
+    <row r="12" spans="1:33" ht="14.25" customHeight="1">
       <c r="A12" s="16"/>
       <c r="B12" s="16" t="s">
         <v>38</v>
@@ -3402,17 +3465,21 @@
       <c r="U12" s="7"/>
       <c r="Z12" s="7"/>
       <c r="AA12" s="33">
-        <v>1996</v>
+        <v>2000</v>
       </c>
       <c r="AB12" s="78"/>
       <c r="AC12" s="33">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="AD12" s="43">
-        <v>1.1990000000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:32" ht="14.25" customHeight="1">
+        <v>1.484</v>
+      </c>
+      <c r="AF12" s="32">
+        <v>33645</v>
+      </c>
+      <c r="AG12" s="60"/>
+    </row>
+    <row r="13" spans="1:33" ht="14.25" customHeight="1">
       <c r="A13" s="16"/>
       <c r="B13" s="16" t="s">
         <v>40</v>
@@ -3446,17 +3513,23 @@
       <c r="U13" s="7"/>
       <c r="Z13" s="7"/>
       <c r="AA13" s="33">
-        <v>1997</v>
-      </c>
-      <c r="AB13" s="33">
-        <v>2500</v>
-      </c>
-      <c r="AC13" s="78"/>
+        <v>2001</v>
+      </c>
+      <c r="AB13" s="78"/>
+      <c r="AC13" s="33">
+        <v>155</v>
+      </c>
       <c r="AD13" s="43">
-        <v>1.1990000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:32" ht="14.25" customHeight="1">
+        <v>1.42</v>
+      </c>
+      <c r="AF13" s="32">
+        <v>34216</v>
+      </c>
+      <c r="AG13" s="60">
+        <v>24.779</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" ht="14.25" customHeight="1">
       <c r="A14" s="16"/>
       <c r="B14" s="16" t="s">
         <v>42</v>
@@ -3490,17 +3563,21 @@
       <c r="U14" s="7"/>
       <c r="Z14" s="7"/>
       <c r="AA14" s="33">
-        <v>1998</v>
+        <v>2002</v>
       </c>
       <c r="AB14" s="78"/>
       <c r="AC14" s="33">
-        <v>140</v>
+        <v>165</v>
       </c>
       <c r="AD14" s="43">
-        <v>1.03</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" ht="14.25" customHeight="1">
+        <v>1.345</v>
+      </c>
+      <c r="AF14" s="32">
+        <v>34894</v>
+      </c>
+      <c r="AG14" s="60"/>
+    </row>
+    <row r="15" spans="1:33" ht="14.25" customHeight="1">
       <c r="A15" s="16"/>
       <c r="B15" s="16" t="s">
         <v>44</v>
@@ -3528,17 +3605,21 @@
       <c r="U15" s="7"/>
       <c r="Z15" s="7"/>
       <c r="AA15" s="33">
-        <v>1999</v>
+        <v>2003</v>
       </c>
       <c r="AB15" s="33">
-        <v>1800</v>
+        <v>830</v>
       </c>
       <c r="AC15" s="78"/>
       <c r="AD15" s="43">
-        <v>1.1359999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32" ht="14.25" customHeight="1">
+        <v>1.5609999999999999</v>
+      </c>
+      <c r="AF15" s="32">
+        <v>35474</v>
+      </c>
+      <c r="AG15" s="60"/>
+    </row>
+    <row r="16" spans="1:33" ht="14.25" customHeight="1">
       <c r="A16" s="16"/>
       <c r="B16" s="16" t="s">
         <v>45</v>
@@ -3566,20 +3647,21 @@
       <c r="U16" s="7"/>
       <c r="Z16" s="7"/>
       <c r="AA16" s="33">
-        <v>2000</v>
+        <v>2004</v>
       </c>
       <c r="AB16" s="78"/>
       <c r="AC16" s="33">
-        <v>150</v>
+        <v>185</v>
       </c>
       <c r="AD16" s="43">
-        <v>1.484</v>
+        <v>1.8520000000000001</v>
       </c>
       <c r="AF16" s="32">
-        <v>33645</v>
-      </c>
-    </row>
-    <row r="17" spans="1:32" ht="14.25" customHeight="1">
+        <v>36325</v>
+      </c>
+      <c r="AG16" s="60"/>
+    </row>
+    <row r="17" spans="1:33" ht="14.25" customHeight="1">
       <c r="A17" s="16"/>
       <c r="B17" s="16" t="s">
         <v>46</v>
@@ -3607,20 +3689,23 @@
       <c r="U17" s="7"/>
       <c r="Z17" s="7"/>
       <c r="AA17" s="33">
-        <v>2001</v>
-      </c>
-      <c r="AB17" s="78"/>
+        <v>2005</v>
+      </c>
+      <c r="AB17" s="33">
+        <v>630</v>
+      </c>
       <c r="AC17" s="33">
-        <v>155</v>
+        <v>195</v>
       </c>
       <c r="AD17" s="43">
-        <v>1.42</v>
+        <v>2.27</v>
       </c>
       <c r="AF17" s="32">
-        <v>34216</v>
-      </c>
-    </row>
-    <row r="18" spans="1:32" ht="14.25" customHeight="1">
+        <v>36526</v>
+      </c>
+      <c r="AG17" s="60"/>
+    </row>
+    <row r="18" spans="1:33" ht="14.25" customHeight="1">
       <c r="A18" s="16"/>
       <c r="B18" s="16" t="s">
         <v>47</v>
@@ -3648,20 +3733,19 @@
       <c r="U18" s="7"/>
       <c r="Z18" s="7"/>
       <c r="AA18" s="33">
-        <v>2002</v>
+        <v>2006</v>
       </c>
       <c r="AB18" s="78"/>
-      <c r="AC18" s="33">
-        <v>165</v>
-      </c>
+      <c r="AC18" s="78"/>
       <c r="AD18" s="43">
-        <v>1.345</v>
+        <v>2.5720000000000001</v>
       </c>
       <c r="AF18" s="32">
-        <v>34894</v>
-      </c>
-    </row>
-    <row r="19" spans="1:32" ht="14.25" customHeight="1">
+        <v>37570</v>
+      </c>
+      <c r="AG18" s="60"/>
+    </row>
+    <row r="19" spans="1:33" ht="14.25" customHeight="1">
       <c r="A19" s="16"/>
       <c r="B19" s="16" t="s">
         <v>48</v>
@@ -3689,20 +3773,19 @@
       <c r="U19" s="7"/>
       <c r="Z19" s="7"/>
       <c r="AA19" s="33">
-        <v>2003</v>
-      </c>
-      <c r="AB19" s="33">
-        <v>830</v>
-      </c>
+        <v>2007</v>
+      </c>
+      <c r="AB19" s="78"/>
       <c r="AC19" s="78"/>
       <c r="AD19" s="43">
-        <v>1.5609999999999999</v>
+        <v>2.7959999999999998</v>
       </c>
       <c r="AF19" s="32">
-        <v>35474</v>
-      </c>
-    </row>
-    <row r="20" spans="1:32" ht="14.25" customHeight="1">
+        <v>38093</v>
+      </c>
+      <c r="AG19" s="60"/>
+    </row>
+    <row r="20" spans="1:33" ht="14.25" customHeight="1">
       <c r="A20" s="16"/>
       <c r="B20" s="16" t="s">
         <v>49</v>
@@ -3730,20 +3813,21 @@
       <c r="U20" s="7"/>
       <c r="Z20" s="7"/>
       <c r="AA20" s="33">
-        <v>2004</v>
+        <v>2008</v>
       </c>
       <c r="AB20" s="78"/>
       <c r="AC20" s="33">
-        <v>185</v>
+        <v>205</v>
       </c>
       <c r="AD20" s="43">
-        <v>1.8520000000000001</v>
+        <v>3.246</v>
       </c>
       <c r="AF20" s="32">
-        <v>36325</v>
-      </c>
-    </row>
-    <row r="21" spans="1:32" ht="14.25" customHeight="1">
+        <v>38188</v>
+      </c>
+      <c r="AG20" s="60"/>
+    </row>
+    <row r="21" spans="1:33" ht="14.25" customHeight="1">
       <c r="A21" s="16"/>
       <c r="B21" s="16" t="s">
         <v>50</v>
@@ -3775,22 +3859,21 @@
       <c r="Y21" s="7"/>
       <c r="Z21" s="7"/>
       <c r="AA21" s="33">
-        <v>2005</v>
-      </c>
-      <c r="AB21" s="33">
-        <v>630</v>
-      </c>
-      <c r="AC21" s="33">
-        <v>195</v>
-      </c>
+        <v>2009</v>
+      </c>
+      <c r="AB21" s="78"/>
+      <c r="AC21" s="78"/>
       <c r="AD21" s="43">
-        <v>2.27</v>
+        <v>2.3530000000000002</v>
       </c>
       <c r="AF21" s="32">
-        <v>36526</v>
-      </c>
-    </row>
-    <row r="22" spans="1:32" ht="14.25" customHeight="1">
+        <v>37814</v>
+      </c>
+      <c r="AG21" s="60">
+        <v>27.943000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" ht="14.25" customHeight="1">
       <c r="A22" s="16"/>
       <c r="B22" s="16" t="s">
         <v>51</v>
@@ -3822,18 +3905,21 @@
       <c r="Y22" s="7"/>
       <c r="Z22" s="7"/>
       <c r="AA22" s="33">
-        <v>2006</v>
-      </c>
-      <c r="AB22" s="78"/>
+        <v>2010</v>
+      </c>
+      <c r="AB22" s="33">
+        <v>370</v>
+      </c>
       <c r="AC22" s="78"/>
       <c r="AD22" s="43">
-        <v>2.5720000000000001</v>
+        <v>2.782</v>
       </c>
       <c r="AF22" s="32">
-        <v>37570</v>
-      </c>
-    </row>
-    <row r="23" spans="1:32" ht="14.25" customHeight="1">
+        <v>38282</v>
+      </c>
+      <c r="AG22" s="60"/>
+    </row>
+    <row r="23" spans="1:33" ht="14.25" customHeight="1">
       <c r="A23" s="16"/>
       <c r="B23" s="16" t="s">
         <v>52</v>
@@ -3865,18 +3951,22 @@
       <c r="Y23" s="7"/>
       <c r="Z23" s="7"/>
       <c r="AA23" s="33">
-        <v>2007</v>
+        <v>2011</v>
       </c>
       <c r="AB23" s="78"/>
       <c r="AC23" s="78"/>
       <c r="AD23" s="43">
-        <v>2.7959999999999998</v>
+        <v>3.5209999999999999</v>
+      </c>
+      <c r="AE23" s="75">
+        <v>7</v>
       </c>
       <c r="AF23" s="32">
-        <v>38093</v>
-      </c>
-    </row>
-    <row r="24" spans="1:32" ht="14.25" customHeight="1">
+        <v>38769</v>
+      </c>
+      <c r="AG23" s="60"/>
+    </row>
+    <row r="24" spans="1:33" ht="14.25" customHeight="1">
       <c r="A24" s="16"/>
       <c r="B24" s="16" t="s">
         <v>53</v>
@@ -3908,20 +3998,22 @@
       <c r="Y24" s="7"/>
       <c r="Z24" s="7"/>
       <c r="AA24" s="33">
-        <v>2008</v>
+        <v>2012</v>
       </c>
       <c r="AB24" s="78"/>
-      <c r="AC24" s="33">
-        <v>205</v>
-      </c>
+      <c r="AC24" s="78"/>
       <c r="AD24" s="43">
-        <v>3.246</v>
+        <v>3.6179999999999999</v>
+      </c>
+      <c r="AE24" s="75">
+        <v>7</v>
       </c>
       <c r="AF24" s="32">
-        <v>38188</v>
-      </c>
-    </row>
-    <row r="25" spans="1:32" ht="14.25" customHeight="1">
+        <v>39732</v>
+      </c>
+      <c r="AG24" s="60"/>
+    </row>
+    <row r="25" spans="1:33" ht="14.25" customHeight="1">
       <c r="A25" s="16"/>
       <c r="B25" s="16" t="s">
         <v>54</v>
@@ -3953,18 +4045,24 @@
       <c r="Y25" s="7"/>
       <c r="Z25" s="7"/>
       <c r="AA25" s="33">
-        <v>2009</v>
+        <v>2013</v>
       </c>
       <c r="AB25" s="78"/>
-      <c r="AC25" s="78"/>
+      <c r="AC25" s="33">
+        <v>240</v>
+      </c>
       <c r="AD25" s="43">
-        <v>2.3530000000000002</v>
+        <v>3.5049999999999999</v>
+      </c>
+      <c r="AE25" s="75">
+        <v>7</v>
       </c>
       <c r="AF25" s="32">
-        <v>37814</v>
-      </c>
-    </row>
-    <row r="26" spans="1:32" ht="14.25" customHeight="1">
+        <v>38947</v>
+      </c>
+      <c r="AG25" s="60"/>
+    </row>
+    <row r="26" spans="1:33" ht="14.25" customHeight="1">
       <c r="A26" s="16"/>
       <c r="B26" s="16" t="s">
         <v>55</v>
@@ -3996,20 +4094,22 @@
       <c r="Y26" s="7"/>
       <c r="Z26" s="7"/>
       <c r="AA26" s="33">
-        <v>2010</v>
-      </c>
-      <c r="AB26" s="33">
-        <v>370</v>
-      </c>
+        <v>2014</v>
+      </c>
+      <c r="AB26" s="78"/>
       <c r="AC26" s="78"/>
       <c r="AD26" s="43">
-        <v>2.782</v>
+        <v>3.3580000000000001</v>
+      </c>
+      <c r="AE26" s="75">
+        <v>10</v>
       </c>
       <c r="AF26" s="32">
-        <v>38282</v>
-      </c>
-    </row>
-    <row r="27" spans="1:32" ht="14.25" customHeight="1">
+        <v>40118</v>
+      </c>
+      <c r="AG26" s="60"/>
+    </row>
+    <row r="27" spans="1:33" ht="14.25" customHeight="1">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -4035,21 +4135,24 @@
       <c r="Y27" s="7"/>
       <c r="Z27" s="7"/>
       <c r="AA27" s="33">
-        <v>2011</v>
-      </c>
-      <c r="AB27" s="78"/>
+        <v>2015</v>
+      </c>
+      <c r="AB27" s="33">
+        <v>350</v>
+      </c>
       <c r="AC27" s="78"/>
       <c r="AD27" s="43">
-        <v>3.5209999999999999</v>
+        <v>2.4289999999999998</v>
       </c>
       <c r="AE27" s="75">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AF27" s="32">
-        <v>38769</v>
-      </c>
-    </row>
-    <row r="28" spans="1:32" ht="14.25" customHeight="1">
+        <v>41383</v>
+      </c>
+      <c r="AG27" s="60"/>
+    </row>
+    <row r="28" spans="1:33" ht="14.25" customHeight="1">
       <c r="A28" s="16"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -4075,21 +4178,20 @@
       <c r="Y28" s="7"/>
       <c r="Z28" s="7"/>
       <c r="AA28" s="33">
-        <v>2012</v>
-      </c>
-      <c r="AB28" s="78"/>
-      <c r="AC28" s="78"/>
+        <v>2016</v>
+      </c>
       <c r="AD28" s="43">
-        <v>3.6179999999999999</v>
+        <v>2.1429999999999998</v>
       </c>
       <c r="AE28" s="75">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AF28" s="32">
-        <v>39732</v>
-      </c>
-    </row>
-    <row r="29" spans="1:32" ht="14.25" customHeight="1">
+        <v>41821</v>
+      </c>
+      <c r="AG28" s="60"/>
+    </row>
+    <row r="29" spans="1:33" ht="14.25" customHeight="1">
       <c r="A29" s="16"/>
       <c r="B29" s="82" t="s">
         <v>56</v>
@@ -4119,23 +4221,22 @@
       <c r="Y29" s="7"/>
       <c r="Z29" s="7"/>
       <c r="AA29" s="33">
-        <v>2013</v>
-      </c>
-      <c r="AB29" s="78"/>
-      <c r="AC29" s="33">
-        <v>240</v>
+        <v>2017</v>
       </c>
       <c r="AD29" s="43">
-        <v>3.5049999999999999</v>
+        <v>2.415</v>
       </c>
       <c r="AE29" s="75">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AF29" s="32">
-        <v>38947</v>
-      </c>
-    </row>
-    <row r="30" spans="1:32" ht="14.25" customHeight="1">
+        <v>42699</v>
+      </c>
+      <c r="AG29" s="60">
+        <v>33.651000000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" ht="14.25" customHeight="1">
       <c r="A30" s="16"/>
       <c r="B30" s="16" t="s">
         <v>57</v>
@@ -4165,21 +4266,20 @@
       <c r="Y30" s="7"/>
       <c r="Z30" s="7"/>
       <c r="AA30" s="33">
-        <v>2014</v>
-      </c>
-      <c r="AB30" s="78"/>
-      <c r="AC30" s="78"/>
+        <v>2018</v>
+      </c>
       <c r="AD30" s="43">
-        <v>3.3580000000000001</v>
+        <v>2.7189999999999999</v>
       </c>
       <c r="AE30" s="75">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="AF30" s="32">
-        <v>40118</v>
-      </c>
-    </row>
-    <row r="31" spans="1:32" ht="14.25" customHeight="1">
+        <v>43886</v>
+      </c>
+      <c r="AG30" s="60"/>
+    </row>
+    <row r="31" spans="1:33" ht="14.25" customHeight="1">
       <c r="A31" s="16"/>
       <c r="B31" s="82" t="s">
         <v>58</v>
@@ -4209,23 +4309,20 @@
       <c r="Y31" s="7"/>
       <c r="Z31" s="7"/>
       <c r="AA31" s="33">
-        <v>2015</v>
-      </c>
-      <c r="AB31" s="33">
-        <v>350</v>
-      </c>
-      <c r="AC31" s="78"/>
+        <v>2019</v>
+      </c>
       <c r="AD31" s="43">
-        <v>2.4289999999999998</v>
+        <v>2.6040000000000001</v>
       </c>
       <c r="AE31" s="75">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="AF31" s="32">
-        <v>41383</v>
-      </c>
-    </row>
-    <row r="32" spans="1:32" ht="14.25" customHeight="1">
+        <v>44644</v>
+      </c>
+      <c r="AG31" s="60"/>
+    </row>
+    <row r="32" spans="1:33" ht="14.25" customHeight="1">
       <c r="A32" s="16"/>
       <c r="B32" s="16" t="s">
         <v>59</v>
@@ -4255,17 +4352,18 @@
       <c r="Y32" s="7"/>
       <c r="Z32" s="7"/>
       <c r="AA32" s="33">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="AD32" s="43">
-        <v>2.1429999999999998</v>
+        <v>2.1680000000000001</v>
       </c>
       <c r="AE32" s="75">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="AF32" s="32">
-        <v>41821</v>
-      </c>
+        <v>47241</v>
+      </c>
+      <c r="AG32" s="60"/>
     </row>
     <row r="33" spans="1:32" ht="14.25" customHeight="1">
       <c r="A33" s="16"/>
@@ -4295,16 +4393,16 @@
       <c r="Y33" s="7"/>
       <c r="Z33" s="7"/>
       <c r="AA33" s="33">
-        <v>2017</v>
+        <v>2021</v>
       </c>
       <c r="AD33" s="43">
-        <v>2.415</v>
+        <v>3.008</v>
       </c>
       <c r="AE33" s="75">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="AF33" s="32">
-        <v>42699</v>
+        <v>48219</v>
       </c>
     </row>
     <row r="34" spans="1:32" ht="14.25" customHeight="1">
@@ -4313,16 +4411,13 @@
       <c r="K34" s="24"/>
       <c r="L34" s="25"/>
       <c r="AA34" s="33">
-        <v>2018</v>
-      </c>
-      <c r="AD34" s="43">
-        <v>2.7189999999999999</v>
+        <v>2022</v>
+      </c>
+      <c r="AD34" s="44">
+        <v>3.9510000000000001</v>
       </c>
       <c r="AE34" s="75">
-        <v>13</v>
-      </c>
-      <c r="AF34" s="32">
-        <v>43886</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:32" ht="19">
@@ -4354,18 +4449,6 @@
       <c r="X35" s="7"/>
       <c r="Y35" s="7"/>
       <c r="Z35" s="7"/>
-      <c r="AA35" s="33">
-        <v>2019</v>
-      </c>
-      <c r="AD35" s="43">
-        <v>2.6040000000000001</v>
-      </c>
-      <c r="AE35" s="75">
-        <v>25</v>
-      </c>
-      <c r="AF35" s="32">
-        <v>44644</v>
-      </c>
     </row>
     <row r="36" spans="1:32" ht="60" customHeight="1">
       <c r="A36" s="27"/>
@@ -4400,18 +4483,6 @@
       <c r="X36" s="7"/>
       <c r="Y36" s="7"/>
       <c r="Z36" s="7"/>
-      <c r="AA36" s="33">
-        <v>2020</v>
-      </c>
-      <c r="AD36" s="43">
-        <v>2.1680000000000001</v>
-      </c>
-      <c r="AE36" s="75">
-        <v>25</v>
-      </c>
-      <c r="AF36" s="32">
-        <v>47241</v>
-      </c>
     </row>
     <row r="37" spans="1:32" ht="14.25" customHeight="1">
       <c r="A37" s="27"/>
@@ -4446,18 +4517,6 @@
       <c r="X37" s="7"/>
       <c r="Y37" s="7"/>
       <c r="Z37" s="7"/>
-      <c r="AA37" s="33">
-        <v>2021</v>
-      </c>
-      <c r="AD37" s="43">
-        <v>3.008</v>
-      </c>
-      <c r="AE37" s="75">
-        <v>30</v>
-      </c>
-      <c r="AF37" s="32">
-        <v>48219</v>
-      </c>
     </row>
     <row r="38" spans="1:32" ht="14.25" customHeight="1">
       <c r="A38" s="27"/>
@@ -4492,15 +4551,6 @@
       <c r="X38" s="7"/>
       <c r="Y38" s="7"/>
       <c r="Z38" s="7"/>
-      <c r="AA38" s="33">
-        <v>2022</v>
-      </c>
-      <c r="AD38" s="44">
-        <v>3.9510000000000001</v>
-      </c>
-      <c r="AE38" s="75">
-        <v>27</v>
-      </c>
     </row>
     <row r="39" spans="1:32" ht="14.25" customHeight="1">
       <c r="A39" s="27"/>
@@ -10611,8 +10661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AY1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D22" sqref="A22:D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>

</xml_diff>